<commit_message>
THAT'S IT???? I GUESS
fazer uns testes, em situações falsas, a testar bem as prioridades etc...
</commit_message>
<xml_diff>
--- a/DATA.xlsx
+++ b/DATA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://estgv-my.sharepoint.com/personal/pv22981_alunos_estgv_ipv_pt/Documents/3 ano/2 semestre/ProjetoFinal/ProjetoFinal3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="124" documentId="11_1E72CB516018D59AD64BB047848AF462F5668C01" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{865B17A8-2272-48DA-A047-4BBB91FAFCD7}"/>
+  <xr:revisionPtr revIDLastSave="138" documentId="11_1E72CB516018D59AD64BB047848AF462F5668C01" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E7BBEF32-DDFA-4F8E-8C86-00C607FD5FC4}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WORKER" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5788" uniqueCount="2072">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5794" uniqueCount="2078">
   <si>
     <t>Skill</t>
   </si>
@@ -6276,6 +6276,24 @@
   </si>
   <si>
     <t>id-1000</t>
+  </si>
+  <si>
+    <t>PRIORITY_APPOINTMENT</t>
+  </si>
+  <si>
+    <t>0.5</t>
+  </si>
+  <si>
+    <t>PRIORITY_CREATION</t>
+  </si>
+  <si>
+    <t>0.9</t>
+  </si>
+  <si>
+    <t>quanto menor o valor maior a prioridade da Atividade, 1 -&gt; Nenhuma prioridade</t>
+  </si>
+  <si>
+    <t>0 -&gt; Prioridade máxima para as Atividades com marcação, 1 -&gt; Nenhuma prioridade para as Ativiades com marcação,  &gt;1 -&gt; prioridade para as Atividades sem marcação</t>
   </si>
 </sst>
 </file>
@@ -6776,7 +6794,7 @@
   </sheetPr>
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -51299,15 +51317,17 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="95.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="96.5546875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -51351,7 +51371,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -51439,8 +51459,31 @@
         <v>26</v>
       </c>
     </row>
+    <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>2072</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>2073</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>2077</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>2074</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>2075</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>2076</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
A usar a API, compor, testes
</commit_message>
<xml_diff>
--- a/DATA.xlsx
+++ b/DATA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://estgv-my.sharepoint.com/personal/pv22981_alunos_estgv_ipv_pt/Documents/3 ano/2 semestre/ProjetoFinal/ProjetoFinal3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="138" documentId="11_1E72CB516018D59AD64BB047848AF462F5668C01" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E7BBEF32-DDFA-4F8E-8C86-00C607FD5FC4}"/>
+  <xr:revisionPtr revIDLastSave="146" documentId="11_1E72CB516018D59AD64BB047848AF462F5668C01" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5EAC3296-6645-4AC5-AC4D-1ACC054F7DB4}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5794" uniqueCount="2078">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5792" uniqueCount="2077">
   <si>
     <t>Skill</t>
   </si>
@@ -6281,19 +6281,16 @@
     <t>PRIORITY_APPOINTMENT</t>
   </si>
   <si>
-    <t>0.5</t>
-  </si>
-  <si>
     <t>PRIORITY_CREATION</t>
   </si>
   <si>
-    <t>0.9</t>
-  </si>
-  <si>
     <t>quanto menor o valor maior a prioridade da Atividade, 1 -&gt; Nenhuma prioridade</t>
   </si>
   <si>
     <t>0 -&gt; Prioridade máxima para as Atividades com marcação, 1 -&gt; Nenhuma prioridade para as Ativiades com marcação,  &gt;1 -&gt; prioridade para as Atividades sem marcação</t>
+  </si>
+  <si>
+    <t>7:00;11:00</t>
   </si>
 </sst>
 </file>
@@ -6832,25 +6829,25 @@
     </row>
     <row r="2" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C2" s="1">
-        <v>74140</v>
+        <v>51380</v>
       </c>
       <c r="D2" t="s">
-        <v>1065</v>
+        <v>4</v>
       </c>
       <c r="E2" s="5">
-        <v>43.502648866636378</v>
+        <v>46.615953294355222</v>
       </c>
       <c r="F2" s="5">
-        <v>0.21340461754543771</v>
+        <v>-0.21034809587029771</v>
       </c>
       <c r="G2" t="s">
-        <v>1062</v>
+        <v>2076</v>
       </c>
     </row>
   </sheetData>
@@ -7291,7 +7288,7 @@
   <dimension ref="A1:G171"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -51320,7 +51317,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -51398,7 +51395,7 @@
         <v>17</v>
       </c>
       <c r="B7" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>18</v>
@@ -51420,7 +51417,7 @@
         <v>21</v>
       </c>
       <c r="B9" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>22</v>
@@ -51431,7 +51428,7 @@
         <v>23</v>
       </c>
       <c r="B10" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>24</v>
@@ -51463,22 +51460,22 @@
       <c r="A13" t="s">
         <v>2072</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>2073</v>
+      <c r="B13" s="2">
+        <v>1</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>2077</v>
+        <v>2075</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>2073</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>2074</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>2075</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>2076</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
imagem melhor, vários clustering
melhorei a parte de mostrar o percurso do Trabalhador

lógica para a escolha do método de clustering
</commit_message>
<xml_diff>
--- a/DATA.xlsx
+++ b/DATA.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jgac0\OneDrive - ESTGV\3 ano\2 semestre\ProjetoFinal\ProjetoFinal3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://estgv-my.sharepoint.com/personal/pv22981_alunos_estgv_ipv_pt/Documents/3 ano/2 semestre/ProjetoFinal/ProjetoFinal3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D3E3769-C4F2-4F21-A8EE-009FFA7E5B85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{5D3E3769-C4F2-4F21-A8EE-009FFA7E5B85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{822CD750-EBFC-40A7-AE2D-356F20F1E4CF}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5792" uniqueCount="2077">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5792" uniqueCount="2076">
   <si>
     <t>Skill</t>
   </si>
@@ -6288,9 +6288,6 @@
   </si>
   <si>
     <t>cost by hour (16)</t>
-  </si>
-  <si>
-    <t>FTTH, FTTHx, Cworks</t>
   </si>
 </sst>
 </file>
@@ -6471,6 +6468,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6834,7 +6835,7 @@
         <v>29720</v>
       </c>
       <c r="D2" t="s">
-        <v>2076</v>
+        <v>1064</v>
       </c>
       <c r="E2" s="5">
         <v>43.523674647031847</v>

</xml_diff>

<commit_message>
Compor o Novo Custo
</commit_message>
<xml_diff>
--- a/DATA.xlsx
+++ b/DATA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://estgv-my.sharepoint.com/personal/pv22981_alunos_estgv_ipv_pt/Documents/3 ano/2 semestre/ProjetoFinal/ProjetoFinal3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_DE8FE7C740A12F1989494C177EFFF2250D6B9552" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="11_DE8FE7C740A12F1989494C177EFFF2250D6B9552" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BC7BEA4E-772E-43B5-8593-4CC0C6B374EA}"/>
   <bookViews>
-    <workbookView xWindow="2172" yWindow="0" windowWidth="19548" windowHeight="12240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WORKER" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3743" uniqueCount="1279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3742" uniqueCount="1277">
   <si>
     <t>Skill</t>
   </si>
@@ -3868,12 +3868,6 @@
   </si>
   <si>
     <t>Worker-170</t>
-  </si>
-  <si>
-    <t>idCentral</t>
-  </si>
-  <si>
-    <t>codPostal</t>
   </si>
 </sst>
 </file>
@@ -4182,6 +4176,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4502,7 +4500,9 @@
   </sheetPr>
   <dimension ref="A1:P12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -4518,25 +4518,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="1" t="s">
         <v>1096</v>
       </c>
-      <c r="B1" s="35" t="s">
-        <v>1277</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1278</v>
-      </c>
-      <c r="D1" s="35" t="s">
+      <c r="B1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1097</v>
       </c>
+      <c r="D1" s="30" t="s">
+        <v>42</v>
+      </c>
       <c r="E1" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="F1" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="G1" s="35" t="s">
+      <c r="F1" s="35" t="s">
         <v>1098</v>
       </c>
     </row>
@@ -4547,19 +4544,16 @@
       <c r="B2" t="s">
         <v>220</v>
       </c>
-      <c r="C2" s="32">
-        <v>97240</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="33">
+        <v>43.974274567555838</v>
       </c>
       <c r="E2" s="33">
-        <v>43.974274567555838</v>
-      </c>
-      <c r="F2" s="33">
         <v>-0.4775894473437714</v>
       </c>
-      <c r="G2" t="s">
+      <c r="F2" t="s">
         <v>1100</v>
       </c>
     </row>
@@ -4589,7 +4583,9 @@
   </sheetPr>
   <dimension ref="A1:F171"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -8031,7 +8027,7 @@
   </sheetPr>
   <dimension ref="A1:M1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -39093,7 +39089,9 @@
   </sheetPr>
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -39222,7 +39220,7 @@
         <v>25</v>
       </c>
       <c r="B11" s="11">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>26</v>

</xml_diff>